<commit_message>
Update PurchaseOrderItem model to allow blank descriptions; add migration and implement Excel worksheet setup functions
</commit_message>
<xml_diff>
--- a/PO_Template.xlsx
+++ b/PO_Template.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Hayes Instrument Service, Inc.</t>
   </si>
@@ -183,40 +183,25 @@
     <t>Notes:</t>
   </si>
   <si>
-    <t>PLEASE ADD DIP SEAL TO ALL THREAD GAUGE</t>
-  </si>
-  <si>
     <t>SUBTOTAL</t>
   </si>
   <si>
     <t>OTHER COSTS:</t>
   </si>
   <si>
-    <t>MAKE CERTIFICATE TO:   GEMS SENSORS INC</t>
-  </si>
-  <si>
     <t>SHIPPING</t>
   </si>
   <si>
     <t>HAYES SHIPPING</t>
   </si>
   <si>
-    <t>CALIBRATE USING 12 MONTH CAL CYCLE - NOTIFY PRIOR TO ANY REPAIR OR ADJUSTMENT</t>
-  </si>
-  <si>
     <t>TAX</t>
   </si>
   <si>
     <t>INBOUND FREIGHT</t>
   </si>
   <si>
-    <t>Calibrate traceable to SI.  Before and after data required.  Calibration must be compliant to:</t>
-  </si>
-  <si>
     <t>TOTAL</t>
-  </si>
-  <si>
-    <t>ANSI/NCSL Z540-1-1994</t>
   </si>
   <si>
     <t>*SHIP/RETURN TO 530 BOSTON RD, BILLERICA, MA 01821 UNLESS OTHERWISE NOTED               **HAYES INSTRUMENT SERVICE T&amp;C'S APPLIES TO ALL ORDERS</t>
@@ -333,7 +318,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -443,36 +428,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -494,19 +449,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -604,12 +546,90 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -711,89 +731,41 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -805,35 +777,98 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1139,8 +1174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2109,13 +2144,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="47.45" customHeight="1">
-      <c r="D1" s="73" t="s">
+      <c r="D1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -2126,13 +2161,13 @@
     <row r="2" spans="2:15" ht="22.9" customHeight="1" thickBot="1">
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
-      <c r="D2" s="74" t="s">
+      <c r="D2" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
       <c r="I2" s="4" t="s">
         <v>3</v>
       </c>
@@ -2145,13 +2180,13 @@
     <row r="3" spans="2:15" ht="15" customHeight="1">
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
-      <c r="D3" s="75" t="s">
+      <c r="D3" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
       <c r="I3" s="19"/>
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
@@ -2159,18 +2194,18 @@
     <row r="4" spans="2:15" ht="18.600000000000001" customHeight="1" thickBot="1">
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
-      <c r="D4" s="76" t="s">
+      <c r="D4" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="76"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
       <c r="I4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="77"/>
-      <c r="K4" s="77"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
       <c r="M4" s="15" t="s">
         <v>8</v>
       </c>
@@ -2178,13 +2213,13 @@
     <row r="5" spans="2:15" ht="14.45" customHeight="1">
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
-      <c r="D5" s="78" t="s">
+      <c r="D5" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="78"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
@@ -2193,10 +2228,10 @@
       </c>
     </row>
     <row r="6" spans="2:15" ht="24.75" customHeight="1">
-      <c r="B6" s="69" t="s">
+      <c r="B6" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="69"/>
+      <c r="C6" s="43"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -2204,11 +2239,11 @@
       <c r="H6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="69" t="s">
+      <c r="I6" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="69"/>
-      <c r="K6" s="69"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
       <c r="N6" s="9" t="s">
         <v>14</v>
       </c>
@@ -2217,20 +2252,20 @@
       </c>
     </row>
     <row r="7" spans="2:15" ht="22.5" customHeight="1" thickBot="1">
-      <c r="B7" s="70"/>
-      <c r="C7" s="70"/>
-      <c r="D7" s="70"/>
-      <c r="E7" s="70"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="71" t="s">
+      <c r="I7" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="71"/>
-      <c r="K7" s="71"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="45"/>
       <c r="N7" s="9" t="s">
         <v>18</v>
       </c>
@@ -2239,18 +2274,18 @@
       </c>
     </row>
     <row r="8" spans="2:15" ht="16.149999999999999" customHeight="1" thickBot="1">
-      <c r="B8" s="64"/>
-      <c r="C8" s="64"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="64"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
       <c r="H8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="72" t="s">
+      <c r="I8" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="J8" s="72"/>
-      <c r="K8" s="72"/>
+      <c r="J8" s="48"/>
+      <c r="K8" s="48"/>
       <c r="N8" s="9" t="s">
         <v>22</v>
       </c>
@@ -2259,10 +2294,10 @@
       </c>
     </row>
     <row r="9" spans="2:15" ht="16.5" customHeight="1" thickBot="1">
-      <c r="B9" s="64"/>
-      <c r="C9" s="64"/>
-      <c r="D9" s="64"/>
-      <c r="E9" s="64"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
       <c r="G9" s="4"/>
       <c r="I9" s="10" t="s">
         <v>24</v>
@@ -2275,18 +2310,18 @@
       </c>
     </row>
     <row r="10" spans="2:15" ht="18" customHeight="1" thickBot="1">
-      <c r="B10" s="64"/>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="64"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
       <c r="H10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I10" s="65" t="s">
+      <c r="I10" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="J10" s="65"/>
-      <c r="K10" s="65"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="49"/>
       <c r="L10" s="11"/>
       <c r="N10" s="9" t="s">
         <v>29</v>
@@ -2299,9 +2334,9 @@
       <c r="B11" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="66"/>
-      <c r="D11" s="66"/>
-      <c r="E11" s="66"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
       <c r="H11" s="13" t="s">
         <v>32</v>
       </c>
@@ -2319,9 +2354,9 @@
       <c r="B12" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="67"/>
-      <c r="D12" s="67"/>
-      <c r="E12" s="67"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
       <c r="F12" s="16"/>
       <c r="G12" s="8" t="s">
         <v>37</v>
@@ -2329,19 +2364,19 @@
       <c r="H12" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="I12" s="68" t="s">
+      <c r="I12" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="J12" s="68"/>
-      <c r="K12" s="68"/>
+      <c r="J12" s="52"/>
+      <c r="K12" s="52"/>
     </row>
     <row r="13" spans="2:15" ht="18" customHeight="1" thickBot="1">
       <c r="B13" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="61"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
       <c r="F13" s="16"/>
       <c r="K13" s="18"/>
       <c r="M13" s="2" t="s">
@@ -2349,9 +2384,9 @@
       </c>
     </row>
     <row r="14" spans="2:15" ht="6.75" customHeight="1">
-      <c r="B14" s="62"/>
-      <c r="C14" s="62"/>
-      <c r="D14" s="62"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="54"/>
       <c r="E14" s="7"/>
       <c r="G14" s="20"/>
       <c r="H14" s="20"/>
@@ -2369,10 +2404,10 @@
       <c r="D15" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="63" t="s">
+      <c r="E15" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="F15" s="63"/>
+      <c r="F15" s="55"/>
       <c r="G15" s="21" t="s">
         <v>46</v>
       </c>
@@ -2382,10 +2417,10 @@
       <c r="I15" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="J15" s="63" t="s">
+      <c r="J15" s="55" t="s">
         <v>49</v>
       </c>
-      <c r="K15" s="63"/>
+      <c r="K15" s="55"/>
       <c r="M15" s="22" t="s">
         <v>50</v>
       </c>
@@ -2400,18 +2435,18 @@
       <c r="B16" s="23"/>
       <c r="C16" s="24"/>
       <c r="D16" s="24"/>
-      <c r="E16" s="53"/>
-      <c r="F16" s="53"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56"/>
       <c r="G16" s="24"/>
       <c r="H16" s="24"/>
       <c r="I16" s="25">
         <v>0</v>
       </c>
-      <c r="J16" s="60">
+      <c r="J16" s="57">
         <f>+I16*D16</f>
         <v>0</v>
       </c>
-      <c r="K16" s="60"/>
+      <c r="K16" s="57"/>
       <c r="L16" s="26"/>
       <c r="M16" s="27"/>
       <c r="N16" s="27"/>
@@ -2419,160 +2454,155 @@
     </row>
     <row r="17" spans="2:15" s="26" customFormat="1" ht="22.15" customHeight="1">
       <c r="B17" s="29"/>
-      <c r="C17" s="24"/>
+      <c r="C17" s="37"/>
       <c r="D17" s="24"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="56"/>
       <c r="G17" s="30"/>
       <c r="H17" s="24"/>
       <c r="I17" s="25">
         <v>0</v>
       </c>
-      <c r="J17" s="60">
+      <c r="J17" s="57">
         <f t="shared" ref="J17:J26" si="0">+I17*D17</f>
         <v>0</v>
       </c>
-      <c r="K17" s="60"/>
+      <c r="K17" s="57"/>
       <c r="M17" s="27"/>
       <c r="N17" s="27"/>
       <c r="O17" s="28"/>
     </row>
     <row r="18" spans="2:15" s="26" customFormat="1" ht="22.15" customHeight="1">
       <c r="B18" s="29"/>
-      <c r="C18" s="24"/>
+      <c r="C18" s="37"/>
       <c r="D18" s="24"/>
-      <c r="E18" s="53"/>
-      <c r="F18" s="53"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="56"/>
       <c r="G18" s="31"/>
       <c r="H18" s="24"/>
       <c r="I18" s="25">
         <v>0</v>
       </c>
-      <c r="J18" s="60">
+      <c r="J18" s="57">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K18" s="60"/>
+      <c r="K18" s="57"/>
       <c r="M18" s="27"/>
       <c r="N18" s="27"/>
       <c r="O18" s="28"/>
     </row>
     <row r="19" spans="2:15" s="26" customFormat="1" ht="22.15" customHeight="1">
       <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
+      <c r="C19" s="37"/>
       <c r="D19" s="24"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="53"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="56"/>
       <c r="G19" s="31"/>
       <c r="H19" s="24"/>
       <c r="I19" s="25">
         <v>0</v>
       </c>
-      <c r="J19" s="60">
+      <c r="J19" s="57">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K19" s="60"/>
+      <c r="K19" s="57"/>
       <c r="M19" s="27"/>
       <c r="N19" s="27"/>
       <c r="O19" s="28"/>
     </row>
     <row r="20" spans="2:15" s="26" customFormat="1" ht="22.15" customHeight="1">
       <c r="B20" s="29"/>
-      <c r="C20" s="29"/>
+      <c r="C20" s="37"/>
       <c r="D20" s="24"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
+      <c r="E20" s="56"/>
+      <c r="F20" s="56"/>
       <c r="G20" s="31"/>
       <c r="H20" s="24"/>
       <c r="I20" s="25">
         <v>0</v>
       </c>
-      <c r="J20" s="60">
+      <c r="J20" s="57">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K20" s="60"/>
+      <c r="K20" s="57"/>
       <c r="M20" s="27"/>
       <c r="N20" s="27"/>
       <c r="O20" s="28"/>
     </row>
     <row r="21" spans="2:15" s="26" customFormat="1" ht="22.15" customHeight="1">
       <c r="B21" s="29"/>
-      <c r="C21" s="29"/>
+      <c r="C21" s="37"/>
       <c r="D21" s="24"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="53"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="56"/>
       <c r="G21" s="31"/>
       <c r="H21" s="24"/>
       <c r="I21" s="25">
         <v>0</v>
       </c>
-      <c r="J21" s="60">
+      <c r="J21" s="57">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K21" s="60"/>
+      <c r="K21" s="57"/>
       <c r="M21" s="27"/>
       <c r="N21" s="27"/>
       <c r="O21" s="28"/>
     </row>
     <row r="22" spans="2:15" s="26" customFormat="1" ht="22.15" customHeight="1">
       <c r="B22" s="29"/>
-      <c r="C22" s="29"/>
+      <c r="C22" s="37"/>
       <c r="D22" s="24"/>
-      <c r="E22" s="53"/>
-      <c r="F22" s="53"/>
+      <c r="E22" s="56"/>
+      <c r="F22" s="56"/>
       <c r="G22" s="31"/>
       <c r="H22" s="24"/>
       <c r="I22" s="25">
         <v>0</v>
       </c>
-      <c r="J22" s="60">
+      <c r="J22" s="57">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K22" s="60"/>
+      <c r="K22" s="57"/>
       <c r="M22" s="27"/>
       <c r="N22" s="27"/>
       <c r="O22" s="28"/>
     </row>
     <row r="23" spans="2:15" s="26" customFormat="1" ht="22.15" customHeight="1">
       <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
+      <c r="C23" s="37"/>
       <c r="D23" s="24"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="53"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="56"/>
       <c r="G23" s="31"/>
       <c r="H23" s="24"/>
       <c r="I23" s="25">
         <v>0</v>
       </c>
-      <c r="J23" s="60">
+      <c r="J23" s="57">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K23" s="60"/>
+      <c r="K23" s="57"/>
       <c r="M23" s="27"/>
       <c r="N23" s="27"/>
       <c r="O23" s="28"/>
     </row>
     <row r="24" spans="2:15" s="26" customFormat="1" ht="22.15" customHeight="1">
       <c r="B24" s="29"/>
-      <c r="C24" s="29"/>
+      <c r="C24" s="37"/>
       <c r="D24" s="24"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="53"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="56"/>
       <c r="G24" s="31"/>
       <c r="H24" s="24"/>
-      <c r="I24" s="25">
-        <v>0</v>
-      </c>
-      <c r="J24" s="60">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K24" s="60"/>
+      <c r="I24" s="73"/>
+      <c r="J24" s="74"/>
+      <c r="K24" s="74"/>
       <c r="M24" s="27"/>
       <c r="N24" s="27"/>
       <c r="O24" s="28"/>
@@ -2581,40 +2611,30 @@
       <c r="B25" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="29"/>
+      <c r="C25" s="37"/>
       <c r="D25" s="24"/>
-      <c r="E25" s="53"/>
-      <c r="F25" s="53"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="56"/>
       <c r="G25" s="31"/>
       <c r="H25" s="24"/>
-      <c r="I25" s="25">
-        <v>0</v>
-      </c>
-      <c r="J25" s="60">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K25" s="60"/>
+      <c r="I25" s="73"/>
+      <c r="J25" s="74"/>
+      <c r="K25" s="74"/>
       <c r="M25" s="27"/>
       <c r="N25" s="27"/>
       <c r="O25" s="28"/>
     </row>
     <row r="26" spans="2:15" s="26" customFormat="1" ht="22.15" customHeight="1" thickBot="1">
       <c r="B26" s="29"/>
-      <c r="C26" s="29"/>
+      <c r="C26" s="37"/>
       <c r="D26" s="24"/>
-      <c r="E26" s="53"/>
-      <c r="F26" s="53"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="56"/>
       <c r="G26" s="31"/>
       <c r="H26" s="24"/>
-      <c r="I26" s="25">
-        <v>0</v>
-      </c>
-      <c r="J26" s="54">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K26" s="54"/>
+      <c r="I26" s="73"/>
+      <c r="J26" s="75"/>
+      <c r="K26" s="75"/>
       <c r="M26" s="27"/>
       <c r="N26" s="27"/>
       <c r="O26" s="28"/>
@@ -2623,170 +2643,160 @@
       <c r="B27" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="55" t="s">
+      <c r="C27" s="68"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="68"/>
+      <c r="F27" s="68"/>
+      <c r="G27" s="68"/>
+      <c r="H27" s="69"/>
+      <c r="I27" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="D27" s="55"/>
-      <c r="E27" s="55"/>
-      <c r="F27" s="55"/>
-      <c r="G27" s="55"/>
-      <c r="H27" s="56"/>
-      <c r="I27" s="33" t="s">
-        <v>56</v>
-      </c>
-      <c r="J27" s="57">
+      <c r="J27" s="76">
         <f>SUM(J16:K26)</f>
         <v>0</v>
       </c>
-      <c r="K27" s="58"/>
+      <c r="K27" s="77"/>
       <c r="M27" s="26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" s="26" customFormat="1" ht="22.15" customHeight="1">
+      <c r="B28" s="70"/>
+      <c r="C28" s="71"/>
+      <c r="D28" s="71"/>
+      <c r="E28" s="71"/>
+      <c r="F28" s="71"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="72"/>
+      <c r="I28" s="34" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="28" spans="2:15" s="26" customFormat="1" ht="22.15" customHeight="1">
-      <c r="B28" s="37" t="s">
+      <c r="J28" s="78">
+        <v>0</v>
+      </c>
+      <c r="K28" s="79"/>
+      <c r="M28" s="35" t="s">
         <v>58</v>
-      </c>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="34" t="s">
-        <v>59</v>
-      </c>
-      <c r="J28" s="59">
-        <v>0</v>
-      </c>
-      <c r="K28" s="59"/>
-      <c r="M28" s="35" t="s">
-        <v>60</v>
       </c>
       <c r="N28" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:15" s="26" customFormat="1" ht="22.15" customHeight="1" thickBot="1">
-      <c r="B29" s="37" t="s">
-        <v>61</v>
-      </c>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="39"/>
+      <c r="B29" s="70"/>
+      <c r="C29" s="71"/>
+      <c r="D29" s="71"/>
+      <c r="E29" s="71"/>
+      <c r="F29" s="71"/>
+      <c r="G29" s="71"/>
+      <c r="H29" s="72"/>
       <c r="I29" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="J29" s="40">
+        <v>59</v>
+      </c>
+      <c r="J29" s="80">
         <v>0</v>
       </c>
-      <c r="K29" s="40"/>
+      <c r="K29" s="81"/>
       <c r="M29" s="35" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="N29" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="2:15" s="26" customFormat="1" ht="21.75" customHeight="1">
-      <c r="B30" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="C30" s="42"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="43"/>
-      <c r="I30" s="44" t="s">
-        <v>65</v>
-      </c>
-      <c r="J30" s="46">
+      <c r="B30" s="58"/>
+      <c r="C30" s="59"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="59"/>
+      <c r="F30" s="59"/>
+      <c r="G30" s="59"/>
+      <c r="H30" s="60"/>
+      <c r="I30" s="82" t="s">
+        <v>61</v>
+      </c>
+      <c r="J30" s="61">
         <f>SUM(J27:K29)</f>
         <v>0</v>
       </c>
-      <c r="K30" s="47"/>
+      <c r="K30" s="62"/>
       <c r="L30" s="15"/>
     </row>
     <row r="31" spans="2:15" s="26" customFormat="1" ht="21.75" customHeight="1" thickBot="1">
-      <c r="B31" s="50" t="s">
-        <v>66</v>
-      </c>
-      <c r="C31" s="51"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="51"/>
-      <c r="F31" s="51"/>
-      <c r="G31" s="51"/>
-      <c r="H31" s="52"/>
-      <c r="I31" s="45"/>
-      <c r="J31" s="48"/>
-      <c r="K31" s="49"/>
+      <c r="B31" s="65"/>
+      <c r="C31" s="66"/>
+      <c r="D31" s="66"/>
+      <c r="E31" s="66"/>
+      <c r="F31" s="66"/>
+      <c r="G31" s="66"/>
+      <c r="H31" s="67"/>
+      <c r="I31" s="83"/>
+      <c r="J31" s="63"/>
+      <c r="K31" s="64"/>
       <c r="L31" s="15"/>
     </row>
     <row r="32" spans="2:15" ht="23.25" customHeight="1">
       <c r="B32" s="15" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="B30:H30"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="J30:K31"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="C27:H27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="B28:H28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="B29:H29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="I7:K7"/>
     <mergeCell ref="D5:H5"/>
     <mergeCell ref="D1:H1"/>
     <mergeCell ref="D2:H2"/>
     <mergeCell ref="D3:H3"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="J4:K4"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="C27:H27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="B28:H28"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="B30:H30"/>
-    <mergeCell ref="I30:I31"/>
-    <mergeCell ref="J30:K31"/>
-    <mergeCell ref="B31:H31"/>
   </mergeCells>
   <dataValidations count="8">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I8:K8">

</xml_diff>